<commit_message>
new data about pib
</commit_message>
<xml_diff>
--- a/Data/data_set_new_cantons.xlsx
+++ b/Data/data_set_new_cantons.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U23"/>
+  <dimension ref="A1:X23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -472,6 +472,21 @@
           <t>distance</t>
         </is>
       </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>poblacion2016</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>pib</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>quartile</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -543,6 +558,17 @@
       <c r="U2" t="n">
         <v>227</v>
       </c>
+      <c r="V2" t="n">
+        <v>29305</v>
+      </c>
+      <c r="W2" t="n">
+        <v>32867.59</v>
+      </c>
+      <c r="X2" t="inlineStr">
+        <is>
+          <t>first quartile</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -614,6 +640,17 @@
       <c r="U3" t="n">
         <v>224</v>
       </c>
+      <c r="V3" t="n">
+        <v>44434</v>
+      </c>
+      <c r="W3" t="n">
+        <v>88617.14</v>
+      </c>
+      <c r="X3" t="inlineStr">
+        <is>
+          <t>second quartile</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -685,6 +722,17 @@
       <c r="U4" t="n">
         <v>153</v>
       </c>
+      <c r="V4" t="n">
+        <v>132041</v>
+      </c>
+      <c r="W4" t="n">
+        <v>288262.31</v>
+      </c>
+      <c r="X4" t="inlineStr">
+        <is>
+          <t>more third quartile</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -756,6 +804,17 @@
       <c r="U5" t="n">
         <v>93</v>
       </c>
+      <c r="V5" t="n">
+        <v>103731</v>
+      </c>
+      <c r="W5" t="n">
+        <v>230106.32</v>
+      </c>
+      <c r="X5" t="inlineStr">
+        <is>
+          <t>more third quartile</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -827,6 +886,17 @@
       <c r="U6" t="n">
         <v>157</v>
       </c>
+      <c r="V6" t="n">
+        <v>24862</v>
+      </c>
+      <c r="W6" t="n">
+        <v>43572.24</v>
+      </c>
+      <c r="X6" t="inlineStr">
+        <is>
+          <t>first quartile</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -898,6 +968,17 @@
       <c r="U7" t="n">
         <v>51</v>
       </c>
+      <c r="V7" t="n">
+        <v>25448</v>
+      </c>
+      <c r="W7" t="n">
+        <v>32581.87</v>
+      </c>
+      <c r="X7" t="inlineStr">
+        <is>
+          <t>first quartile</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -969,6 +1050,17 @@
       <c r="U8" t="n">
         <v>188</v>
       </c>
+      <c r="V8" t="n">
+        <v>24302</v>
+      </c>
+      <c r="W8" t="n">
+        <v>240970.74</v>
+      </c>
+      <c r="X8" t="inlineStr">
+        <is>
+          <t>more third quartile</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1040,6 +1132,17 @@
       <c r="U9" t="n">
         <v>238</v>
       </c>
+      <c r="V9" t="n">
+        <v>74804</v>
+      </c>
+      <c r="W9" t="n">
+        <v>116284.87</v>
+      </c>
+      <c r="X9" t="inlineStr">
+        <is>
+          <t>third quartile</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1111,6 +1214,17 @@
       <c r="U10" t="n">
         <v>181</v>
       </c>
+      <c r="V10" t="n">
+        <v>19300</v>
+      </c>
+      <c r="W10" t="n">
+        <v>146767.18</v>
+      </c>
+      <c r="X10" t="inlineStr">
+        <is>
+          <t>third quartile</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1182,6 +1296,17 @@
       <c r="U11" t="n">
         <v>195</v>
       </c>
+      <c r="V11" t="n">
+        <v>253441</v>
+      </c>
+      <c r="W11" t="n">
+        <v>1849299.44</v>
+      </c>
+      <c r="X11" t="inlineStr">
+        <is>
+          <t>more third quartile</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1253,6 +1378,17 @@
       <c r="U12" t="n">
         <v>195</v>
       </c>
+      <c r="V12" t="n">
+        <v>92234</v>
+      </c>
+      <c r="W12" t="n">
+        <v>659769.89</v>
+      </c>
+      <c r="X12" t="inlineStr">
+        <is>
+          <t>more third quartile</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1324,6 +1460,17 @@
       <c r="U13" t="n">
         <v>238</v>
       </c>
+      <c r="V13" t="n">
+        <v>4589</v>
+      </c>
+      <c r="W13" t="n">
+        <v>13358.26</v>
+      </c>
+      <c r="X13" t="inlineStr">
+        <is>
+          <t>first quartile</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1395,6 +1542,17 @@
       <c r="U14" t="n">
         <v>278</v>
       </c>
+      <c r="V14" t="n">
+        <v>37929</v>
+      </c>
+      <c r="W14" t="n">
+        <v>52329.28</v>
+      </c>
+      <c r="X14" t="inlineStr">
+        <is>
+          <t>second quartile</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1466,6 +1624,17 @@
       <c r="U15" t="n">
         <v>0</v>
       </c>
+      <c r="V15" t="n">
+        <v>61193</v>
+      </c>
+      <c r="W15" t="n">
+        <v>128480.48</v>
+      </c>
+      <c r="X15" t="inlineStr">
+        <is>
+          <t>third quartile</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1537,6 +1706,17 @@
       <c r="U16" t="n">
         <v>235</v>
       </c>
+      <c r="V16" t="n">
+        <v>30546</v>
+      </c>
+      <c r="W16" t="n">
+        <v>42251.74</v>
+      </c>
+      <c r="X16" t="inlineStr">
+        <is>
+          <t>first quartile</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1608,6 +1788,17 @@
       <c r="U17" t="n">
         <v>182</v>
       </c>
+      <c r="V17" t="n">
+        <v>310582</v>
+      </c>
+      <c r="W17" t="n">
+        <v>1580563.51</v>
+      </c>
+      <c r="X17" t="inlineStr">
+        <is>
+          <t>more third quartile</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1679,6 +1870,17 @@
       <c r="U18" t="n">
         <v>294</v>
       </c>
+      <c r="V18" t="n">
+        <v>23342</v>
+      </c>
+      <c r="W18" t="n">
+        <v>42533.56</v>
+      </c>
+      <c r="X18" t="inlineStr">
+        <is>
+          <t>first quartile</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1750,6 +1952,17 @@
       <c r="U19" t="n">
         <v>167</v>
       </c>
+      <c r="V19" t="n">
+        <v>36470</v>
+      </c>
+      <c r="W19" t="n">
+        <v>56999.28</v>
+      </c>
+      <c r="X19" t="inlineStr">
+        <is>
+          <t>second quartile</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1821,6 +2034,17 @@
       <c r="U20" t="n">
         <v>109</v>
       </c>
+      <c r="V20" t="n">
+        <v>24139</v>
+      </c>
+      <c r="W20" t="n">
+        <v>47652.57</v>
+      </c>
+      <c r="X20" t="inlineStr">
+        <is>
+          <t>second quartile</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1892,6 +2116,17 @@
       <c r="U21" t="n">
         <v>203</v>
       </c>
+      <c r="V21" t="n">
+        <v>48920</v>
+      </c>
+      <c r="W21" t="n">
+        <v>62482.19</v>
+      </c>
+      <c r="X21" t="inlineStr">
+        <is>
+          <t>second quartile</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1963,6 +2198,17 @@
       <c r="U22" t="n">
         <v>211</v>
       </c>
+      <c r="V22" t="n">
+        <v>61553</v>
+      </c>
+      <c r="W22" t="n">
+        <v>205934.49</v>
+      </c>
+      <c r="X22" t="inlineStr">
+        <is>
+          <t>third quartile</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -2033,6 +2279,17 @@
       </c>
       <c r="U23" t="n">
         <v>157</v>
+      </c>
+      <c r="V23" t="n">
+        <v>41524</v>
+      </c>
+      <c r="W23" t="n">
+        <v>100939.6</v>
+      </c>
+      <c r="X23" t="inlineStr">
+        <is>
+          <t>third quartile</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modifique stata do 2
</commit_message>
<xml_diff>
--- a/Data/data_set_new_cantons.xlsx
+++ b/Data/data_set_new_cantons.xlsx
@@ -562,7 +562,7 @@
         <v>29305</v>
       </c>
       <c r="W2" t="n">
-        <v>32867.59</v>
+        <v>30861.45</v>
       </c>
       <c r="X2" t="inlineStr">
         <is>
@@ -644,7 +644,7 @@
         <v>44434</v>
       </c>
       <c r="W3" t="n">
-        <v>88617.14</v>
+        <v>87608.38</v>
       </c>
       <c r="X3" t="inlineStr">
         <is>
@@ -726,7 +726,7 @@
         <v>132041</v>
       </c>
       <c r="W4" t="n">
-        <v>288262.31</v>
+        <v>309613.32</v>
       </c>
       <c r="X4" t="inlineStr">
         <is>
@@ -808,7 +808,7 @@
         <v>103731</v>
       </c>
       <c r="W5" t="n">
-        <v>230106.32</v>
+        <v>214081.99</v>
       </c>
       <c r="X5" t="inlineStr">
         <is>
@@ -890,7 +890,7 @@
         <v>24862</v>
       </c>
       <c r="W6" t="n">
-        <v>43572.24</v>
+        <v>47076.8</v>
       </c>
       <c r="X6" t="inlineStr">
         <is>
@@ -972,7 +972,7 @@
         <v>25448</v>
       </c>
       <c r="W7" t="n">
-        <v>32581.87</v>
+        <v>28885.1</v>
       </c>
       <c r="X7" t="inlineStr">
         <is>
@@ -1054,11 +1054,11 @@
         <v>24302</v>
       </c>
       <c r="W8" t="n">
-        <v>240970.74</v>
+        <v>188411.03</v>
       </c>
       <c r="X8" t="inlineStr">
         <is>
-          <t>more third quartile</t>
+          <t>third quartile</t>
         </is>
       </c>
     </row>
@@ -1136,7 +1136,7 @@
         <v>74804</v>
       </c>
       <c r="W9" t="n">
-        <v>116284.87</v>
+        <v>120517.63</v>
       </c>
       <c r="X9" t="inlineStr">
         <is>
@@ -1218,7 +1218,7 @@
         <v>19300</v>
       </c>
       <c r="W10" t="n">
-        <v>146767.18</v>
+        <v>114987.25</v>
       </c>
       <c r="X10" t="inlineStr">
         <is>
@@ -1300,7 +1300,7 @@
         <v>253441</v>
       </c>
       <c r="W11" t="n">
-        <v>1849299.44</v>
+        <v>1934032.42</v>
       </c>
       <c r="X11" t="inlineStr">
         <is>
@@ -1382,7 +1382,7 @@
         <v>92234</v>
       </c>
       <c r="W12" t="n">
-        <v>659769.89</v>
+        <v>634454.0600000001</v>
       </c>
       <c r="X12" t="inlineStr">
         <is>
@@ -1464,7 +1464,7 @@
         <v>4589</v>
       </c>
       <c r="W13" t="n">
-        <v>13358.26</v>
+        <v>12801.68</v>
       </c>
       <c r="X13" t="inlineStr">
         <is>
@@ -1546,7 +1546,7 @@
         <v>37929</v>
       </c>
       <c r="W14" t="n">
-        <v>52329.28</v>
+        <v>50041.66</v>
       </c>
       <c r="X14" t="inlineStr">
         <is>
@@ -1628,7 +1628,7 @@
         <v>61193</v>
       </c>
       <c r="W15" t="n">
-        <v>128480.48</v>
+        <v>132225.73</v>
       </c>
       <c r="X15" t="inlineStr">
         <is>
@@ -1710,7 +1710,7 @@
         <v>30546</v>
       </c>
       <c r="W16" t="n">
-        <v>42251.74</v>
+        <v>42710.61</v>
       </c>
       <c r="X16" t="inlineStr">
         <is>
@@ -1792,7 +1792,7 @@
         <v>310582</v>
       </c>
       <c r="W17" t="n">
-        <v>1580563.51</v>
+        <v>1604021.07</v>
       </c>
       <c r="X17" t="inlineStr">
         <is>
@@ -1874,7 +1874,7 @@
         <v>23342</v>
       </c>
       <c r="W18" t="n">
-        <v>42533.56</v>
+        <v>40219.7</v>
       </c>
       <c r="X18" t="inlineStr">
         <is>
@@ -1956,7 +1956,7 @@
         <v>36470</v>
       </c>
       <c r="W19" t="n">
-        <v>56999.28</v>
+        <v>48927.17</v>
       </c>
       <c r="X19" t="inlineStr">
         <is>
@@ -2038,7 +2038,7 @@
         <v>24139</v>
       </c>
       <c r="W20" t="n">
-        <v>47652.57</v>
+        <v>58949.94</v>
       </c>
       <c r="X20" t="inlineStr">
         <is>
@@ -2120,7 +2120,7 @@
         <v>48920</v>
       </c>
       <c r="W21" t="n">
-        <v>62482.19</v>
+        <v>47916.46</v>
       </c>
       <c r="X21" t="inlineStr">
         <is>
@@ -2202,11 +2202,11 @@
         <v>61553</v>
       </c>
       <c r="W22" t="n">
-        <v>205934.49</v>
+        <v>189664.68</v>
       </c>
       <c r="X22" t="inlineStr">
         <is>
-          <t>third quartile</t>
+          <t>more third quartile</t>
         </is>
       </c>
     </row>
@@ -2284,7 +2284,7 @@
         <v>41524</v>
       </c>
       <c r="W23" t="n">
-        <v>100939.6</v>
+        <v>108451.44</v>
       </c>
       <c r="X23" t="inlineStr">
         <is>

</xml_diff>